<commit_message>
updates to roruns script
</commit_message>
<xml_diff>
--- a/src/roruns.xlsx
+++ b/src/roruns.xlsx
@@ -1,26 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markh\Documents\swot-error\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66BF1B30-281A-4987-ABE5-B75CD1CACEEA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D23C3E0-6AF7-460D-9EA3-A0FF0DB2F5CA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20760" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="roruns" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="38">
   <si>
     <t>outroot</t>
   </si>
@@ -127,13 +135,19 @@
     <t>$SACDIR9</t>
   </si>
   <si>
-    <t>preseg_iter</t>
+    <t>gdem_name</t>
+  </si>
+  <si>
+    <t>gdem_truth.LeftSwath.nc</t>
+  </si>
+  <si>
+    <t>gdem_preproc.nc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -967,11 +981,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,8 +1076,8 @@
       <c r="L2" t="s">
         <v>17</v>
       </c>
-      <c r="M2">
-        <v>0</v>
+      <c r="M2" t="s">
+        <v>36</v>
       </c>
       <c r="N2" t="s">
         <v>18</v>
@@ -1108,8 +1122,8 @@
       <c r="L3" t="s">
         <v>17</v>
       </c>
-      <c r="M3">
-        <v>0</v>
+      <c r="M3" t="s">
+        <v>36</v>
       </c>
       <c r="N3" t="s">
         <v>18</v>
@@ -1154,8 +1168,8 @@
       <c r="L4" t="s">
         <v>23</v>
       </c>
-      <c r="M4">
-        <v>0</v>
+      <c r="M4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1197,8 +1211,8 @@
       <c r="L5" t="s">
         <v>26</v>
       </c>
-      <c r="M5">
-        <v>0</v>
+      <c r="M5" t="s">
+        <v>36</v>
       </c>
       <c r="N5" t="s">
         <v>27</v>
@@ -1243,8 +1257,8 @@
       <c r="L6" t="s">
         <v>26</v>
       </c>
-      <c r="M6">
-        <v>0</v>
+      <c r="M6" t="s">
+        <v>36</v>
       </c>
       <c r="N6" t="s">
         <v>27</v>
@@ -1289,8 +1303,8 @@
       <c r="L7" t="s">
         <v>23</v>
       </c>
-      <c r="M7">
-        <v>0</v>
+      <c r="M7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1332,8 +1346,8 @@
       <c r="L8" t="s">
         <v>23</v>
       </c>
-      <c r="M8">
-        <v>0</v>
+      <c r="M8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1375,8 +1389,8 @@
       <c r="L9" t="s">
         <v>26</v>
       </c>
-      <c r="M9">
-        <v>0</v>
+      <c r="M9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -1418,8 +1432,8 @@
       <c r="L10" t="s">
         <v>26</v>
       </c>
-      <c r="M10">
-        <v>0</v>
+      <c r="M10" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -1461,8 +1475,8 @@
       <c r="L11" t="s">
         <v>23</v>
       </c>
-      <c r="M11">
-        <v>0</v>
+      <c r="M11" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1504,8 +1518,8 @@
       <c r="L12" t="s">
         <v>23</v>
       </c>
-      <c r="M12">
-        <v>0</v>
+      <c r="M12" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1547,8 +1561,8 @@
       <c r="L13" t="s">
         <v>26</v>
       </c>
-      <c r="M13">
-        <v>0</v>
+      <c r="M13" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -1590,8 +1604,8 @@
       <c r="L14" t="s">
         <v>26</v>
       </c>
-      <c r="M14">
-        <v>0</v>
+      <c r="M14" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -1633,8 +1647,8 @@
       <c r="L15" t="s">
         <v>23</v>
       </c>
-      <c r="M15">
-        <v>0</v>
+      <c r="M15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1676,8 +1690,8 @@
       <c r="L16" t="s">
         <v>23</v>
       </c>
-      <c r="M16">
-        <v>0</v>
+      <c r="M16" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -1719,8 +1733,8 @@
       <c r="L17" t="s">
         <v>26</v>
       </c>
-      <c r="M17">
-        <v>0</v>
+      <c r="M17" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -1762,8 +1776,8 @@
       <c r="L18" t="s">
         <v>26</v>
       </c>
-      <c r="M18">
-        <v>0</v>
+      <c r="M18" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -1805,8 +1819,8 @@
       <c r="L19" t="s">
         <v>23</v>
       </c>
-      <c r="M19">
-        <v>0</v>
+      <c r="M19" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -1848,8 +1862,8 @@
       <c r="L20" t="s">
         <v>17</v>
       </c>
-      <c r="M20">
-        <v>1</v>
+      <c r="M20" t="s">
+        <v>37</v>
       </c>
       <c r="N20" t="s">
         <v>18</v>
@@ -1894,8 +1908,8 @@
       <c r="L21" t="s">
         <v>17</v>
       </c>
-      <c r="M21">
-        <v>1</v>
+      <c r="M21" t="s">
+        <v>37</v>
       </c>
       <c r="N21" t="s">
         <v>18</v>
@@ -1940,8 +1954,8 @@
       <c r="L22" t="s">
         <v>23</v>
       </c>
-      <c r="M22">
-        <v>1</v>
+      <c r="M22" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -1983,8 +1997,8 @@
       <c r="L23" t="s">
         <v>26</v>
       </c>
-      <c r="M23">
-        <v>1</v>
+      <c r="M23" t="s">
+        <v>37</v>
       </c>
       <c r="N23" t="s">
         <v>27</v>
@@ -2029,8 +2043,8 @@
       <c r="L24" t="s">
         <v>26</v>
       </c>
-      <c r="M24">
-        <v>1</v>
+      <c r="M24" t="s">
+        <v>37</v>
       </c>
       <c r="N24" t="s">
         <v>27</v>
@@ -2075,8 +2089,8 @@
       <c r="L25" t="s">
         <v>23</v>
       </c>
-      <c r="M25">
-        <v>1</v>
+      <c r="M25" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -2118,8 +2132,8 @@
       <c r="L26" t="s">
         <v>23</v>
       </c>
-      <c r="M26">
-        <v>1</v>
+      <c r="M26" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -2161,8 +2175,8 @@
       <c r="L27" t="s">
         <v>26</v>
       </c>
-      <c r="M27">
-        <v>1</v>
+      <c r="M27" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -2204,8 +2218,8 @@
       <c r="L28" t="s">
         <v>26</v>
       </c>
-      <c r="M28">
-        <v>1</v>
+      <c r="M28" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -2247,8 +2261,8 @@
       <c r="L29" t="s">
         <v>23</v>
       </c>
-      <c r="M29">
-        <v>1</v>
+      <c r="M29" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -2290,8 +2304,8 @@
       <c r="L30" t="s">
         <v>23</v>
       </c>
-      <c r="M30">
-        <v>1</v>
+      <c r="M30" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -2333,8 +2347,8 @@
       <c r="L31" t="s">
         <v>26</v>
       </c>
-      <c r="M31">
-        <v>1</v>
+      <c r="M31" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -2376,8 +2390,8 @@
       <c r="L32" t="s">
         <v>26</v>
       </c>
-      <c r="M32">
-        <v>1</v>
+      <c r="M32" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -2419,8 +2433,8 @@
       <c r="L33" t="s">
         <v>23</v>
       </c>
-      <c r="M33">
-        <v>1</v>
+      <c r="M33" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -2462,8 +2476,8 @@
       <c r="L34" t="s">
         <v>23</v>
       </c>
-      <c r="M34">
-        <v>1</v>
+      <c r="M34" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -2505,8 +2519,8 @@
       <c r="L35" t="s">
         <v>26</v>
       </c>
-      <c r="M35">
-        <v>1</v>
+      <c r="M35" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -2548,8 +2562,8 @@
       <c r="L36" t="s">
         <v>26</v>
       </c>
-      <c r="M36">
-        <v>1</v>
+      <c r="M36" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -2591,8 +2605,8 @@
       <c r="L37" t="s">
         <v>23</v>
       </c>
-      <c r="M37">
-        <v>1</v>
+      <c r="M37" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>